<commit_message>
mb write - part 1
</commit_message>
<xml_diff>
--- a/Snap7/src/tags/mb-tags-s1-d1.xlsx
+++ b/Snap7/src/tags/mb-tags-s1-d1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbystrzycki\Desktop\Snap7\src\tags\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{799E1CA7-18E0-4D33-BCDC-A9D904B2F890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95DD3F0-0C38-4D04-A39D-7FC1701123FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21750" yWindow="2250" windowWidth="14685" windowHeight="11910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MB-Tags" sheetId="25" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="27">
   <si>
     <t>INDEX</t>
   </si>
@@ -637,7 +637,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,10 +724,10 @@
         <v>5</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>10</v>
@@ -743,6 +743,18 @@
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -754,10 +766,18 @@
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="G7" s="4"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -769,6 +789,18 @@
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -780,10 +812,18 @@
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="G9" s="4"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>

</xml_diff>

<commit_message>
mb write - part 2
</commit_message>
<xml_diff>
--- a/Snap7/src/tags/mb-tags-s1-d1.xlsx
+++ b/Snap7/src/tags/mb-tags-s1-d1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbystrzycki\Desktop\Snap7\src\tags\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95DD3F0-0C38-4D04-A39D-7FC1701123FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F1D5FF-116C-42FB-AB41-F94F9B47745F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21750" yWindow="2250" windowWidth="14685" windowHeight="11910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MB-Tags" sheetId="25" r:id="rId1"/>
@@ -637,7 +637,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,7 +699,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="1">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -721,16 +721,16 @@
         <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G5" s="4"/>
       <c r="I5" s="1"/>
@@ -790,7 +790,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -799,7 +799,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G8" s="2"/>
       <c r="I8" s="1"/>
@@ -813,7 +813,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -822,7 +822,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G9" s="4"/>
       <c r="I9" s="1"/>

</xml_diff>